<commit_message>
learnt about conditional operators/case statements
</commit_message>
<xml_diff>
--- a/Learning/Udemy/Ultimate MySQL Bootcamp/MySQL-Ultimate-MySQL-Bootcamp.xlsx
+++ b/Learning/Udemy/Ultimate MySQL Bootcamp/MySQL-Ultimate-MySQL-Bootcamp.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23322"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{376BBC0E-9B2F-495C-8D91-CD9C1090EE81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{23AF5869-D71E-4910-876E-01D204F4C473}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="164">
   <si>
     <t>SQL Commands</t>
   </si>
@@ -46,6 +46,9 @@
     <t>set sql_mode='';</t>
   </si>
   <si>
+    <t>cast()</t>
+  </si>
+  <si>
     <t>// start the CLI</t>
   </si>
   <si>
@@ -422,13 +425,106 @@
   </si>
   <si>
     <t>where &lt;column_nameA&gt; like "___"</t>
+  </si>
+  <si>
+    <t>OPERATORS</t>
+  </si>
+  <si>
+    <t>CASE STATEMENTS</t>
+  </si>
+  <si>
+    <t>// LOGICALS OPERATORS</t>
+  </si>
+  <si>
+    <t>// case statements</t>
+  </si>
+  <si>
+    <t>// NOT EQUAL TO !=</t>
+  </si>
+  <si>
+    <t>select title, released_year,</t>
+  </si>
+  <si>
+    <t>where &lt;column_nameA&gt; != value;</t>
+  </si>
+  <si>
+    <t>case</t>
+  </si>
+  <si>
+    <t>when released_year &gt;= 2000 then 'Modern lit'</t>
+  </si>
+  <si>
+    <t>// NOT LIKE</t>
+  </si>
+  <si>
+    <t>else '20th century lit'</t>
+  </si>
+  <si>
+    <t>where &lt;column_nameA&gt; not like "W%";</t>
+  </si>
+  <si>
+    <t>end as Genre</t>
+  </si>
+  <si>
+    <t>from books_store;</t>
+  </si>
+  <si>
+    <t>// GREATER THAN &gt;= EQUAL TO</t>
+  </si>
+  <si>
+    <t>// 'A' = 'a' -&gt; true (case doesnt matter)</t>
+  </si>
+  <si>
+    <t>where &lt;column_nameA&gt; &gt;= VALUE;</t>
+  </si>
+  <si>
+    <t>// LESS THAN &lt;= EQUAL TO</t>
+  </si>
+  <si>
+    <t>where &lt;column_nameA&gt; &lt;= VALUE;</t>
+  </si>
+  <si>
+    <t>// AND - OR (COMBINE)</t>
+  </si>
+  <si>
+    <t>where &lt;column_nameA&gt; &lt;= VALUE AND &lt;column_nameB&gt; like '%VALUE%';</t>
+  </si>
+  <si>
+    <t>where &lt;column_nameA&gt; &lt;= VALUE OR &lt;column_nameB&gt; like '%VALUE%';</t>
+  </si>
+  <si>
+    <t>// BETWEEN - NOT BETWEEN</t>
+  </si>
+  <si>
+    <t># for date-time use cast()</t>
+  </si>
+  <si>
+    <t>where &lt;column_nameB&gt; between value1 AND value2;</t>
+  </si>
+  <si>
+    <t>where &lt;column_nameB&gt; not between value1 AND value2;</t>
+  </si>
+  <si>
+    <t>// IN / NOT IN - (USE WITH %)</t>
+  </si>
+  <si>
+    <t>where &lt;column_nameA&gt; IN ('valueA', 'valueB', 'valueC')</t>
+  </si>
+  <si>
+    <t>where &lt;column_nameA&gt; NOT IN ('valueA', 'valueB', 'valueC')</t>
+  </si>
+  <si>
+    <t>where &lt;column_nameA&gt; OPERATOR value AND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;column_nameB&gt; % 2 != 0 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -499,6 +595,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222B35"/>
+      <name val="Consolas"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Consolas"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -520,7 +650,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -563,30 +693,10 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -657,41 +767,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -704,23 +802,37 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1036,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:J79"/>
+  <dimension ref="A2:J123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="G74" sqref="G74"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1056,12 +1168,12 @@
     <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:10" ht="15.75">
+      <c r="B2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="28"/>
-      <c r="I2" s="29" t="s">
+      <c r="H2" s="18"/>
+      <c r="I2" s="19" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1069,16 +1181,14 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="2:10">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="39"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="37" t="s">
+      <c r="E4" s="33"/>
+      <c r="G4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -1086,664 +1196,965 @@
       </c>
     </row>
     <row r="5" spans="2:10">
-      <c r="B5" s="5"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-      <c r="G5" s="7"/>
+      <c r="B5" s="36"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="5"/>
+      <c r="G5" s="4"/>
+      <c r="I5" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="2:10">
-      <c r="B6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="G6" s="11" t="s">
+      <c r="D6" s="23" t="s">
         <v>8</v>
       </c>
+      <c r="E6" s="7"/>
+      <c r="G6" s="10" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="2:10">
-      <c r="B7" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="9" t="s">
+      <c r="B7" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="G7" s="11" t="s">
+      <c r="D7" s="23" t="s">
         <v>11</v>
       </c>
+      <c r="E7" s="7"/>
+      <c r="G7" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="I7" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:10">
-      <c r="B8" s="13"/>
-      <c r="D8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="10"/>
-      <c r="G8" s="14" t="s">
+      <c r="B8" s="9"/>
+      <c r="D8" s="23" t="s">
         <v>14</v>
       </c>
+      <c r="E8" s="7"/>
+      <c r="G8" s="8" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="2:10">
-      <c r="B9" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="9" t="s">
+      <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="G9" s="14" t="s">
+      <c r="D9" s="23" t="s">
         <v>17</v>
       </c>
+      <c r="E9" s="7"/>
+      <c r="G9" s="8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="2:10">
-      <c r="B10" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="16" t="s">
+      <c r="B10" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="G10" s="14" t="s">
+      <c r="D10" s="24" t="s">
         <v>20</v>
       </c>
+      <c r="E10" s="7"/>
+      <c r="G10" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="I10" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="2:10">
-      <c r="B11" s="13"/>
-      <c r="D11" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="10"/>
-      <c r="G11" s="14" t="s">
+      <c r="B11" s="9"/>
+      <c r="D11" s="24" t="s">
         <v>24</v>
       </c>
+      <c r="E11" s="7"/>
+      <c r="G11" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="2:10">
-      <c r="B12" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="16" t="s">
+      <c r="B12" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="G12" s="11"/>
+      <c r="D12" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="G12" s="10"/>
       <c r="I12" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="2:10">
-      <c r="B13" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="16" t="s">
+      <c r="B13" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="G13" s="11" t="s">
+      <c r="D13" s="24" t="s">
         <v>30</v>
       </c>
+      <c r="E13" s="7"/>
+      <c r="G13" s="10" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="14" spans="2:10">
-      <c r="B14" s="13"/>
-      <c r="D14" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="10"/>
-      <c r="G14" s="14" t="s">
+      <c r="B14" s="9"/>
+      <c r="D14" s="25" t="s">
         <v>32</v>
       </c>
+      <c r="E14" s="7"/>
+      <c r="G14" s="8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="15" spans="2:10">
-      <c r="B15" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="9" t="s">
+      <c r="B15" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="G15" s="10"/>
+      <c r="D15" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="2:10">
-      <c r="B16" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="16" t="s">
+      <c r="B16" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="10"/>
-      <c r="G16" s="10"/>
+      <c r="D16" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="B17" s="13"/>
-      <c r="D17" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="10"/>
-      <c r="G17" s="10"/>
+      <c r="B17" s="9"/>
+      <c r="D17" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="B18" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="16" t="s">
+      <c r="B18" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="10"/>
-      <c r="G18" s="10"/>
+      <c r="D18" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="G18" s="9"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="B19" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="16" t="s">
+      <c r="B19" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="10"/>
-      <c r="G19" s="10"/>
+      <c r="D19" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="G19" s="9"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="B20" s="18"/>
-      <c r="E20" s="10"/>
-      <c r="G20" s="10"/>
+      <c r="B20" s="11"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="7"/>
+      <c r="G20" s="9"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="B21" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="9" t="s">
+      <c r="B21" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="10"/>
-      <c r="G21" s="10"/>
+      <c r="D21" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="G21" s="9"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="28"/>
-      <c r="B22" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="16" t="s">
+      <c r="A22" s="18"/>
+      <c r="B22" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="10"/>
-      <c r="G22" s="10"/>
+      <c r="D22" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="G22" s="9"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="B23" s="19"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="22"/>
+      <c r="B23" s="12"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="13"/>
+      <c r="G23" s="17"/>
     </row>
     <row r="26" spans="1:7">
       <c r="B26" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="37" t="s">
+      <c r="D26" s="32" t="s">
         <v>48</v>
       </c>
+      <c r="E26" s="33"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="B27" s="5"/>
-      <c r="D27" s="6"/>
+      <c r="B27" s="4"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="7"/>
       <c r="F27" s="31"/>
-      <c r="G27" s="7"/>
+      <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="B28" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="F28" s="32"/>
-      <c r="G28" s="10"/>
+      <c r="B28" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="20"/>
+      <c r="E28" s="7"/>
+      <c r="G28" s="9"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="B29" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="23" t="s">
+      <c r="B29" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F29" s="32"/>
-      <c r="G29" s="33" t="s">
+      <c r="D29" s="29" t="s">
         <v>52</v>
       </c>
+      <c r="E29" s="7"/>
+      <c r="G29" s="14" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" s="7"/>
+      <c r="G30" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="B31" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" s="7"/>
+      <c r="G31" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="B32" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" s="7"/>
+      <c r="G32" s="28"/>
+    </row>
+    <row r="33" spans="2:7">
+      <c r="B33" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" s="20"/>
+      <c r="E33" s="7"/>
+      <c r="G33" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7">
+      <c r="B34" s="10"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="7"/>
+      <c r="G34" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7">
+      <c r="B35" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F30" s="32"/>
-      <c r="G30" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="B31" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="F31" s="32"/>
-      <c r="G31" s="14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="B32" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="F32" s="32"/>
-      <c r="G32" s="34"/>
-    </row>
-    <row r="33" spans="2:7">
-      <c r="B33" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="F33" s="32"/>
-      <c r="G33" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7">
-      <c r="B34" s="15"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7">
-      <c r="B35" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="F35" s="32"/>
-      <c r="G35" s="10"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="7"/>
+      <c r="G35" s="9"/>
     </row>
     <row r="36" spans="2:7">
-      <c r="B36" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="F36" s="32"/>
-      <c r="G36" s="10"/>
+      <c r="B36" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" s="20"/>
+      <c r="E36" s="7"/>
+      <c r="G36" s="9"/>
     </row>
     <row r="37" spans="2:7">
-      <c r="B37" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="F37" s="32"/>
-      <c r="G37" s="10"/>
+      <c r="B37" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" s="20"/>
+      <c r="E37" s="7"/>
+      <c r="G37" s="9"/>
     </row>
     <row r="38" spans="2:7">
-      <c r="B38" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F38" s="32"/>
-      <c r="G38" s="10"/>
+      <c r="B38" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" s="20"/>
+      <c r="E38" s="7"/>
+      <c r="G38" s="9"/>
     </row>
     <row r="39" spans="2:7">
-      <c r="B39" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="F39" s="32"/>
-      <c r="G39" s="10"/>
+      <c r="B39" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="20"/>
+      <c r="E39" s="7"/>
+      <c r="G39" s="9"/>
     </row>
     <row r="40" spans="2:7">
-      <c r="B40" s="15"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="7"/>
+      <c r="G40" s="9"/>
     </row>
     <row r="41" spans="2:7">
-      <c r="B41" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="F41" s="32"/>
-      <c r="G41" s="10"/>
+      <c r="B41" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" s="20"/>
+      <c r="E41" s="7"/>
+      <c r="G41" s="9"/>
     </row>
     <row r="42" spans="2:7">
-      <c r="B42" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="F42" s="32"/>
-      <c r="G42" s="10"/>
+      <c r="B42" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="20"/>
+      <c r="E42" s="7"/>
+      <c r="G42" s="9"/>
     </row>
     <row r="43" spans="2:7">
-      <c r="B43" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="F43" s="32"/>
-      <c r="G43" s="10"/>
+      <c r="B43" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" s="20"/>
+      <c r="E43" s="7"/>
+      <c r="G43" s="9"/>
     </row>
     <row r="44" spans="2:7">
-      <c r="B44" s="26"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="22"/>
+      <c r="B44" s="16"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="13"/>
+      <c r="G44" s="17"/>
     </row>
     <row r="47" spans="2:7">
       <c r="B47" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D47" s="3" t="s">
         <v>72</v>
       </c>
+      <c r="D47" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="E47" s="33"/>
       <c r="G47" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" spans="2:7">
-      <c r="B48" s="5"/>
-      <c r="D48" s="13"/>
-      <c r="G48" s="13"/>
+      <c r="B48" s="4"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="7"/>
+      <c r="G48" s="9"/>
     </row>
     <row r="49" spans="2:7">
-      <c r="B49" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="D49" s="15" t="s">
+      <c r="B49" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G49" s="15" t="s">
+      <c r="D49" s="23" t="s">
         <v>76</v>
       </c>
+      <c r="E49" s="7"/>
+      <c r="G49" s="10" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="50" spans="2:7">
-      <c r="B50" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="D50" s="25" t="s">
+      <c r="B50" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="G50" s="25" t="s">
+      <c r="D50" s="30" t="s">
         <v>79</v>
       </c>
+      <c r="E50" s="7"/>
+      <c r="G50" s="15" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="51" spans="2:7">
-      <c r="B51" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="D51" s="13"/>
-      <c r="G51" s="25" t="s">
+      <c r="B51" s="15" t="s">
         <v>81</v>
       </c>
+      <c r="D51" s="20"/>
+      <c r="E51" s="7"/>
+      <c r="G51" s="15" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="52" spans="2:7">
-      <c r="B52" s="13"/>
-      <c r="D52" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="G52" s="25" t="s">
+      <c r="B52" s="9"/>
+      <c r="D52" s="23" t="s">
         <v>83</v>
       </c>
+      <c r="E52" s="7"/>
+      <c r="G52" s="15" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="53" spans="2:7">
-      <c r="B53" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D53" s="25" t="s">
+      <c r="B53" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="G53" s="13"/>
+      <c r="D53" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="E53" s="7"/>
+      <c r="G53" s="9"/>
     </row>
     <row r="54" spans="2:7">
-      <c r="B54" s="25" t="s">
+      <c r="B54" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D54" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="E54" s="7"/>
+      <c r="G54" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7">
+      <c r="B55" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D55" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="E55" s="7"/>
+      <c r="G55" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D54" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="G54" s="15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7">
-      <c r="B55" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="D55" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="G55" s="12" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="56" spans="2:7">
-      <c r="B56" s="25" t="s">
+      <c r="B56" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D56" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="E56" s="7"/>
+      <c r="G56" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7">
+      <c r="B57" s="9"/>
+      <c r="D57" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="E57" s="7"/>
+      <c r="G57" s="9"/>
+    </row>
+    <row r="58" spans="2:7">
+      <c r="B58" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D58" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="D56" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="G56" s="12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="57" spans="2:7">
-      <c r="B57" s="13"/>
-      <c r="D57" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="G57" s="13"/>
-    </row>
-    <row r="58" spans="2:7">
-      <c r="B58" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="D58" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="G58" s="12" t="s">
-        <v>95</v>
+      <c r="E58" s="7"/>
+      <c r="G58" s="8" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="59" spans="2:7">
-      <c r="B59" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="D59" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="G59" s="12" t="s">
+      <c r="B59" s="15" t="s">
         <v>97</v>
       </c>
+      <c r="D59" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="E59" s="7"/>
+      <c r="G59" s="8" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="60" spans="2:7">
-      <c r="B60" s="13"/>
-      <c r="D60" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="G60" s="13"/>
+      <c r="B60" s="9"/>
+      <c r="D60" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E60" s="7"/>
+      <c r="G60" s="9"/>
     </row>
     <row r="61" spans="2:7">
-      <c r="B61" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="D61" s="13" t="s">
+      <c r="B61" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="G61" s="15" t="s">
+      <c r="D61" s="20" t="s">
         <v>101</v>
       </c>
+      <c r="E61" s="7"/>
+      <c r="G61" s="10" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="62" spans="2:7">
-      <c r="B62" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="D62" s="13"/>
-      <c r="G62" s="12" t="s">
+      <c r="B62" s="15" t="s">
         <v>103</v>
       </c>
+      <c r="D62" s="20"/>
+      <c r="E62" s="7"/>
+      <c r="G62" s="8" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="63" spans="2:7">
-      <c r="B63" s="13"/>
-      <c r="D63" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="G63" s="12" t="s">
+      <c r="B63" s="9"/>
+      <c r="D63" s="23" t="s">
         <v>105</v>
       </c>
+      <c r="E63" s="7"/>
+      <c r="G63" s="8" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="64" spans="2:7">
-      <c r="B64" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="D64" s="13" t="s">
+      <c r="B64" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="G64" s="13"/>
+      <c r="D64" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E64" s="7"/>
+      <c r="G64" s="9"/>
     </row>
     <row r="65" spans="2:7">
-      <c r="B65" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="D65" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="G65" s="15" t="s">
+      <c r="B65" s="15" t="s">
         <v>109</v>
       </c>
+      <c r="D65" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="E65" s="7"/>
+      <c r="G65" s="10" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="66" spans="2:7">
-      <c r="B66" s="13"/>
-      <c r="D66" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="G66" s="12" t="s">
+      <c r="B66" s="9"/>
+      <c r="D66" s="30" t="s">
         <v>111</v>
       </c>
+      <c r="E66" s="7"/>
+      <c r="G66" s="8" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="67" spans="2:7">
-      <c r="B67" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="D67" s="13" t="s">
+      <c r="B67" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="G67" s="12" t="s">
+      <c r="D67" s="20" t="s">
         <v>114</v>
       </c>
+      <c r="E67" s="7"/>
+      <c r="G67" s="8" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="68" spans="2:7">
-      <c r="B68" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="D68" s="25" t="s">
+      <c r="B68" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="G68" s="13" t="s">
+      <c r="D68" s="30" t="s">
         <v>117</v>
       </c>
+      <c r="E68" s="7"/>
+      <c r="G68" s="9" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="69" spans="2:7">
-      <c r="B69" s="13"/>
-      <c r="D69" s="25" t="s">
+      <c r="B69" s="9"/>
+      <c r="D69" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="E69" s="7"/>
+      <c r="G69" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7">
+      <c r="B70" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D70" s="30"/>
+      <c r="E70" s="7"/>
+      <c r="G70" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="G69" s="12" t="s">
+    </row>
+    <row r="71" spans="2:7">
+      <c r="B71" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="D71" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="E71" s="7"/>
+      <c r="G71" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7">
+      <c r="B72" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D72" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="E72" s="7"/>
+      <c r="G72" s="9"/>
+    </row>
+    <row r="73" spans="2:7">
+      <c r="B73" s="15"/>
+      <c r="D73" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="E73" s="7"/>
+      <c r="G73" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7">
+      <c r="B74" s="17"/>
+      <c r="D74" s="30" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="70" spans="2:7">
-      <c r="B70" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="D70" s="25"/>
-      <c r="G70" s="13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="71" spans="2:7">
-      <c r="B71" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="D71" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="G71" s="12" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="72" spans="2:7">
-      <c r="B72" s="25" t="s">
-        <v>124</v>
-      </c>
-      <c r="D72" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="G72" s="13"/>
-    </row>
-    <row r="73" spans="2:7">
-      <c r="B73" s="25"/>
-      <c r="D73" s="13" t="s">
+      <c r="E74" s="7"/>
+      <c r="G74" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7">
+      <c r="D75" s="30"/>
+      <c r="E75" s="7"/>
+      <c r="G75" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7">
+      <c r="D76" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="G73" s="15" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="74" spans="2:7">
-      <c r="B74" s="27"/>
-      <c r="D74" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="G74" s="12" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="75" spans="2:7">
-      <c r="D75" s="25"/>
-      <c r="G75" s="12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="76" spans="2:7">
-      <c r="D76" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="G76" s="13"/>
+      <c r="E76" s="7"/>
+      <c r="G76" s="9"/>
     </row>
     <row r="77" spans="2:7">
-      <c r="D77" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="G77" s="13"/>
+      <c r="D77" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="E77" s="7"/>
+      <c r="G77" s="9"/>
     </row>
     <row r="78" spans="2:7">
-      <c r="D78" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="G78" s="13"/>
+      <c r="D78" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="E78" s="7"/>
+      <c r="G78" s="9"/>
     </row>
     <row r="79" spans="2:7">
-      <c r="D79" s="27"/>
-      <c r="G79" s="27"/>
+      <c r="D79" s="21"/>
+      <c r="E79" s="13"/>
+      <c r="G79" s="17"/>
+    </row>
+    <row r="82" spans="2:4">
+      <c r="B82" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4">
+      <c r="B83" s="9"/>
+      <c r="D83" s="9"/>
+    </row>
+    <row r="84" spans="2:4">
+      <c r="B84" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="D84" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4">
+      <c r="B85" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="D85" s="10"/>
+    </row>
+    <row r="86" spans="2:4">
+      <c r="B86" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D86" s="15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4">
+      <c r="B87" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="D87" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4">
+      <c r="B88" s="10"/>
+      <c r="D88" s="15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4">
+      <c r="B89" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D89" s="15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4">
+      <c r="B90" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D90" s="15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4">
+      <c r="B91" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="D91" s="15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4">
+      <c r="B92" s="15"/>
+      <c r="D92" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4">
+      <c r="B93" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D93" s="10"/>
+    </row>
+    <row r="94" spans="2:4">
+      <c r="B94" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D94" s="10"/>
+    </row>
+    <row r="95" spans="2:4">
+      <c r="B95" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D95" s="15"/>
+    </row>
+    <row r="96" spans="2:4">
+      <c r="B96" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D96" s="15"/>
+    </row>
+    <row r="97" spans="2:4">
+      <c r="B97" s="9"/>
+      <c r="D97" s="9"/>
+    </row>
+    <row r="98" spans="2:4">
+      <c r="B98" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D98" s="10"/>
+    </row>
+    <row r="99" spans="2:4">
+      <c r="B99" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D99" s="15"/>
+    </row>
+    <row r="100" spans="2:4">
+      <c r="B100" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="D100" s="15"/>
+    </row>
+    <row r="101" spans="2:4">
+      <c r="B101" s="15"/>
+      <c r="D101" s="15"/>
+    </row>
+    <row r="102" spans="2:4">
+      <c r="B102" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D102" s="10"/>
+    </row>
+    <row r="103" spans="2:4">
+      <c r="B103" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D103" s="15"/>
+    </row>
+    <row r="104" spans="2:4">
+      <c r="B104" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D104" s="15"/>
+    </row>
+    <row r="105" spans="2:4">
+      <c r="B105" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D105" s="15"/>
+    </row>
+    <row r="106" spans="2:4">
+      <c r="B106" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="D106" s="15"/>
+    </row>
+    <row r="107" spans="2:4">
+      <c r="B107" s="15"/>
+      <c r="D107" s="15"/>
+    </row>
+    <row r="108" spans="2:4">
+      <c r="B108" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="D108" s="10"/>
+    </row>
+    <row r="109" spans="2:4">
+      <c r="B109" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="D109" s="9"/>
+    </row>
+    <row r="110" spans="2:4">
+      <c r="B110" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D110" s="15"/>
+    </row>
+    <row r="111" spans="2:4">
+      <c r="B111" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="D111" s="15"/>
+    </row>
+    <row r="112" spans="2:4">
+      <c r="B112" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D112" s="15"/>
+    </row>
+    <row r="113" spans="2:4">
+      <c r="B113" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="D113" s="15"/>
+    </row>
+    <row r="114" spans="2:4">
+      <c r="B114" s="9"/>
+      <c r="D114" s="9"/>
+    </row>
+    <row r="115" spans="2:4">
+      <c r="B115" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="D115" s="10"/>
+    </row>
+    <row r="116" spans="2:4">
+      <c r="B116" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D116" s="15"/>
+    </row>
+    <row r="117" spans="2:4">
+      <c r="B117" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="D117" s="15"/>
+    </row>
+    <row r="118" spans="2:4">
+      <c r="B118" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D118" s="15"/>
+    </row>
+    <row r="119" spans="2:4">
+      <c r="B119" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="D119" s="15"/>
+    </row>
+    <row r="120" spans="2:4">
+      <c r="B120" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D120" s="15"/>
+    </row>
+    <row r="121" spans="2:4">
+      <c r="B121" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D121" s="15"/>
+    </row>
+    <row r="122" spans="2:4">
+      <c r="B122" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="D122" s="15"/>
+    </row>
+    <row r="123" spans="2:4">
+      <c r="B123" s="17"/>
+      <c r="D123" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D47:E47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
learnt about joins in mysql
</commit_message>
<xml_diff>
--- a/Learning/Udemy/Ultimate MySQL Bootcamp/MySQL-Ultimate-MySQL-Bootcamp.xlsx
+++ b/Learning/Udemy/Ultimate MySQL Bootcamp/MySQL-Ultimate-MySQL-Bootcamp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23322"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23413"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23AF5869-D71E-4910-876E-01D204F4C473}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{329E8DE9-53B7-470F-A5BA-62B036E74E8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SQL - Basic Commands" sheetId="1" r:id="rId1"/>
+    <sheet name="SQL - Commands" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="165">
   <si>
     <t>SQL Commands</t>
   </si>
@@ -130,7 +130,7 @@
     <t>insert into &lt;table_name&gt;() values();</t>
   </si>
   <si>
-    <t>// deleting created database (careful with this command)</t>
+    <t>// deleting created database (carefull with this command)</t>
   </si>
   <si>
     <t>// lists the current table in particular database</t>
@@ -385,36 +385,36 @@
     <t xml:space="preserve">(or) </t>
   </si>
   <si>
+    <t>where &lt;column_name&gt; = (select max(&lt;column_nameA&gt;) from &lt;table_name&gt;)</t>
+  </si>
+  <si>
+    <t>// UPPER-LOWER CASE</t>
+  </si>
+  <si>
+    <t>UPPER('TEXT')</t>
+  </si>
+  <si>
+    <t>// LIKE (WILD CARDS) - % | _ | \</t>
+  </si>
+  <si>
+    <t>order by &lt;column_name&gt; desc limit 1;</t>
+  </si>
+  <si>
+    <t>LOWER('TEXT')</t>
+  </si>
+  <si>
+    <t>select &lt;column_nameA&gt;, &lt;column_nameB&gt; from &lt;table_name&gt;</t>
+  </si>
+  <si>
+    <t>(or) "any-letter%" | "%any-letter" | "%" | "%\%%" | "% %" (it has a space) - This works with texts</t>
+  </si>
+  <si>
+    <t>// sum / average (with 4 decimal count)</t>
+  </si>
+  <si>
     <t>where &lt;column_nameA&gt; like "%any-letter%"</t>
   </si>
   <si>
-    <t>where &lt;column_name&gt; = (select max(&lt;column_nameA&gt;) from &lt;table_name&gt;)</t>
-  </si>
-  <si>
-    <t>// UPPER-LOWER CASE</t>
-  </si>
-  <si>
-    <t>UPPER('TEXT')</t>
-  </si>
-  <si>
-    <t>// LIKE (WILD CARDS) - % | _ | \</t>
-  </si>
-  <si>
-    <t>order by &lt;column_name&gt; desc limit 1;</t>
-  </si>
-  <si>
-    <t>LOWER('TEXT')</t>
-  </si>
-  <si>
-    <t>select &lt;column_nameA&gt;, &lt;column_nameB&gt; from &lt;table_name&gt;</t>
-  </si>
-  <si>
-    <t>(or) "any-letter%" | "%any-letter" | "%" | "%\%%" | "% %" (it has a space) - This works with texts</t>
-  </si>
-  <si>
-    <t>// sum / average (with 4 decimal count)</t>
-  </si>
-  <si>
     <t>select sum(&lt;column_name&gt;) from &lt;table_name&gt;</t>
   </si>
   <si>
@@ -433,6 +433,9 @@
     <t>CASE STATEMENTS</t>
   </si>
   <si>
+    <t>RELATIONSHIPS</t>
+  </si>
+  <si>
     <t>// LOGICALS OPERATORS</t>
   </si>
   <si>
@@ -445,12 +448,12 @@
     <t>select title, released_year,</t>
   </si>
   <si>
+    <t>case</t>
+  </si>
+  <si>
     <t>where &lt;column_nameA&gt; != value;</t>
   </si>
   <si>
-    <t>case</t>
-  </si>
-  <si>
     <t>when released_year &gt;= 2000 then 'Modern lit'</t>
   </si>
   <si>
@@ -460,10 +463,10 @@
     <t>else '20th century lit'</t>
   </si>
   <si>
+    <t>end as Genre</t>
+  </si>
+  <si>
     <t>where &lt;column_nameA&gt; not like "W%";</t>
-  </si>
-  <si>
-    <t>end as Genre</t>
   </si>
   <si>
     <t>from books_store;</t>
@@ -524,7 +527,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -551,12 +554,6 @@
       <name val="Consolas"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF0D0D0D"/>
       <name val="Calibri"/>
@@ -581,37 +578,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF222B35"/>
-      <name val="Consolas"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0D0D0D"/>
-      <name val="Consolas"/>
     </font>
     <font>
       <b/>
@@ -625,6 +597,49 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF305496"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF548235"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF305496"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF2F75B5"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -767,31 +782,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -804,34 +814,62 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1150,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89"/>
+    <sheetView tabSelected="1" topLeftCell="B79" workbookViewId="0">
+      <selection activeCell="G92" sqref="G84:G92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1168,100 +1206,102 @@
     <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="15.75">
-      <c r="B2" s="27" t="s">
+    <row r="2" spans="1:10" ht="15.75">
+      <c r="B2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="19" t="s">
+      <c r="H2" s="15"/>
+      <c r="I2" s="16" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:10">
+    <row r="3" spans="1:10">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="2:10">
-      <c r="B4" s="37" t="s">
+    <row r="4" spans="1:10">
+      <c r="B4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="33"/>
-      <c r="G4" s="3" t="s">
+      <c r="E4" s="43"/>
+      <c r="G4" s="31" t="s">
         <v>4</v>
       </c>
+      <c r="H4" s="30"/>
       <c r="I4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
-      <c r="B5" s="36"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="5"/>
-      <c r="G5" s="4"/>
+    <row r="5" spans="1:10">
+      <c r="B5" s="24"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="4"/>
+      <c r="G5" s="3"/>
       <c r="I5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
-      <c r="B6" s="6" t="s">
+    <row r="6" spans="1:10">
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="G6" s="10" t="s">
+      <c r="E6" s="6"/>
+      <c r="G6" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
-      <c r="B7" s="34" t="s">
+    <row r="7" spans="1:10">
+      <c r="A7" s="15"/>
+      <c r="B7" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="G7" s="10" t="s">
+      <c r="E7" s="6"/>
+      <c r="G7" s="5" t="s">
         <v>12</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
-      <c r="B8" s="9"/>
-      <c r="D8" s="23" t="s">
+    <row r="8" spans="1:10">
+      <c r="B8" s="7"/>
+      <c r="D8" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="G8" s="8" t="s">
+      <c r="E8" s="6"/>
+      <c r="G8" s="28" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
-      <c r="B9" s="6" t="s">
+    <row r="9" spans="1:10">
+      <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="G9" s="8" t="s">
+      <c r="E9" s="6"/>
+      <c r="G9" s="28" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
-      <c r="B10" s="35" t="s">
+    <row r="10" spans="1:10">
+      <c r="B10" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="G10" s="8" t="s">
+      <c r="E10" s="6"/>
+      <c r="G10" s="28" t="s">
         <v>21</v>
       </c>
       <c r="I10" s="2" t="s">
@@ -1271,890 +1311,980 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
-      <c r="B11" s="9"/>
-      <c r="D11" s="24" t="s">
+    <row r="11" spans="1:10">
+      <c r="B11" s="7"/>
+      <c r="D11" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="G11" s="8" t="s">
+      <c r="E11" s="6"/>
+      <c r="G11" s="28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
-      <c r="B12" s="6" t="s">
+    <row r="12" spans="1:10">
+      <c r="B12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="G12" s="10"/>
+      <c r="E12" s="6"/>
+      <c r="G12" s="8"/>
       <c r="I12" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="2:10">
-      <c r="B13" s="35" t="s">
+    <row r="13" spans="1:10">
+      <c r="B13" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="G13" s="10" t="s">
+      <c r="E13" s="6"/>
+      <c r="G13" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
-      <c r="B14" s="9"/>
-      <c r="D14" s="25" t="s">
+    <row r="14" spans="1:10">
+      <c r="B14" s="7"/>
+      <c r="D14" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="G14" s="8" t="s">
+      <c r="E14" s="6"/>
+      <c r="G14" s="28" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="2:10">
-      <c r="B15" s="6" t="s">
+    <row r="15" spans="1:10">
+      <c r="B15" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="D15" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="G15" s="9"/>
-    </row>
-    <row r="16" spans="2:10">
-      <c r="B16" s="35" t="s">
+      <c r="E15" s="6"/>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="B16" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="G16" s="9"/>
+      <c r="E16" s="6"/>
+      <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="B17" s="9"/>
-      <c r="D17" s="23" t="s">
+      <c r="B17" s="7"/>
+      <c r="D17" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="G17" s="9"/>
+      <c r="E17" s="6"/>
+      <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="D18" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="G18" s="9"/>
+      <c r="E18" s="6"/>
+      <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="D19" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="G19" s="9"/>
+      <c r="E19" s="6"/>
+      <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="B20" s="11"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="7"/>
-      <c r="G20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="6"/>
+      <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="D21" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="G21" s="9"/>
+      <c r="E21" s="6"/>
+      <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="18"/>
-      <c r="B22" s="35" t="s">
+      <c r="A22" s="15"/>
+      <c r="B22" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="24" t="s">
+      <c r="D22" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="G22" s="9"/>
+      <c r="E22" s="6"/>
+      <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="B23" s="12"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="13"/>
-      <c r="G23" s="17"/>
+      <c r="B23" s="10"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="11"/>
+      <c r="G23" s="14"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="32" t="s">
+      <c r="D26" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="33"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="3" t="s">
+      <c r="E26" s="45"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="31" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="B27" s="4"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="4"/>
+      <c r="B27" s="3"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="20"/>
-      <c r="E28" s="7"/>
-      <c r="G28" s="9"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="6"/>
+      <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="29" t="s">
+      <c r="D29" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="E29" s="7"/>
-      <c r="G29" s="14" t="s">
+      <c r="E29" s="6"/>
+      <c r="G29" s="33" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="23" t="s">
+      <c r="D30" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="7"/>
-      <c r="G30" s="10" t="s">
+      <c r="E30" s="6"/>
+      <c r="G30" s="5" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="24" t="s">
+      <c r="D31" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="E31" s="7"/>
-      <c r="G31" s="8" t="s">
+      <c r="E31" s="6"/>
+      <c r="G31" s="28" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="24" t="s">
+      <c r="D32" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="E32" s="7"/>
-      <c r="G32" s="28"/>
+      <c r="E32" s="6"/>
+      <c r="G32" s="21"/>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="D33" s="20"/>
-      <c r="E33" s="7"/>
-      <c r="G33" s="10" t="s">
+      <c r="D33" s="27"/>
+      <c r="E33" s="6"/>
+      <c r="G33" s="5" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="34" spans="2:7">
-      <c r="B34" s="10"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="7"/>
-      <c r="G34" s="8" t="s">
+      <c r="B34" s="8"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="6"/>
+      <c r="G34" s="28" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="35" spans="2:7">
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="D35" s="20"/>
-      <c r="E35" s="7"/>
-      <c r="G35" s="9"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="6"/>
+      <c r="G35" s="7"/>
     </row>
     <row r="36" spans="2:7">
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D36" s="20"/>
-      <c r="E36" s="7"/>
-      <c r="G36" s="9"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="6"/>
+      <c r="G36" s="7"/>
     </row>
     <row r="37" spans="2:7">
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D37" s="20"/>
-      <c r="E37" s="7"/>
-      <c r="G37" s="9"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="6"/>
+      <c r="G37" s="7"/>
     </row>
     <row r="38" spans="2:7">
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="D38" s="20"/>
-      <c r="E38" s="7"/>
-      <c r="G38" s="9"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="6"/>
+      <c r="G38" s="7"/>
     </row>
     <row r="39" spans="2:7">
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="D39" s="20"/>
-      <c r="E39" s="7"/>
-      <c r="G39" s="9"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="6"/>
+      <c r="G39" s="7"/>
     </row>
     <row r="40" spans="2:7">
-      <c r="B40" s="10"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="7"/>
-      <c r="G40" s="9"/>
+      <c r="B40" s="8"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="6"/>
+      <c r="G40" s="7"/>
     </row>
     <row r="41" spans="2:7">
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="D41" s="20"/>
-      <c r="E41" s="7"/>
-      <c r="G41" s="9"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="6"/>
+      <c r="G41" s="7"/>
     </row>
     <row r="42" spans="2:7">
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D42" s="20"/>
-      <c r="E42" s="7"/>
-      <c r="G42" s="9"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="6"/>
+      <c r="G42" s="7"/>
     </row>
     <row r="43" spans="2:7">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="D43" s="20"/>
-      <c r="E43" s="7"/>
-      <c r="G43" s="9"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="6"/>
+      <c r="G43" s="7"/>
     </row>
     <row r="44" spans="2:7">
-      <c r="B44" s="16"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="13"/>
-      <c r="G44" s="17"/>
+      <c r="B44" s="13"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="11"/>
+      <c r="G44" s="14"/>
     </row>
     <row r="47" spans="2:7">
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="D47" s="32" t="s">
+      <c r="D47" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="E47" s="33"/>
-      <c r="G47" s="3" t="s">
+      <c r="E47" s="45"/>
+      <c r="G47" s="31" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="48" spans="2:7">
-      <c r="B48" s="4"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="7"/>
-      <c r="G48" s="9"/>
+      <c r="B48" s="3"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="6"/>
+      <c r="G48" s="7"/>
     </row>
     <row r="49" spans="2:7">
-      <c r="B49" s="10" t="s">
+      <c r="B49" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D49" s="23" t="s">
+      <c r="D49" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="E49" s="7"/>
-      <c r="G49" s="10" t="s">
+      <c r="E49" s="6"/>
+      <c r="G49" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="50" spans="2:7">
-      <c r="B50" s="15" t="s">
+      <c r="B50" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="D50" s="30" t="s">
+      <c r="D50" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="E50" s="7"/>
-      <c r="G50" s="15" t="s">
+      <c r="E50" s="6"/>
+      <c r="G50" s="32" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="51" spans="2:7">
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="D51" s="20"/>
-      <c r="E51" s="7"/>
-      <c r="G51" s="15" t="s">
+      <c r="D51" s="17"/>
+      <c r="E51" s="6"/>
+      <c r="G51" s="32" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="52" spans="2:7">
-      <c r="B52" s="9"/>
-      <c r="D52" s="23" t="s">
+      <c r="B52" s="7"/>
+      <c r="D52" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="E52" s="7"/>
-      <c r="G52" s="15" t="s">
+      <c r="E52" s="6"/>
+      <c r="G52" s="32" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="53" spans="2:7">
-      <c r="B53" s="10" t="s">
+      <c r="B53" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D53" s="30" t="s">
+      <c r="D53" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="E53" s="7"/>
-      <c r="G53" s="9"/>
+      <c r="E53" s="6"/>
+      <c r="G53" s="7"/>
     </row>
     <row r="54" spans="2:7">
-      <c r="B54" s="15" t="s">
+      <c r="B54" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="D54" s="30" t="s">
+      <c r="D54" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="E54" s="7"/>
-      <c r="G54" s="10" t="s">
+      <c r="E54" s="6"/>
+      <c r="G54" s="5" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="55" spans="2:7">
-      <c r="B55" s="15" t="s">
+      <c r="B55" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="D55" s="20" t="s">
+      <c r="D55" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="E55" s="7"/>
-      <c r="G55" s="8" t="s">
+      <c r="E55" s="6"/>
+      <c r="G55" s="28" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="56" spans="2:7">
-      <c r="B56" s="15" t="s">
+      <c r="B56" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="D56" s="30" t="s">
+      <c r="D56" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="E56" s="7"/>
-      <c r="G56" s="8" t="s">
+      <c r="E56" s="6"/>
+      <c r="G56" s="28" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="57" spans="2:7">
-      <c r="B57" s="9"/>
-      <c r="D57" s="30" t="s">
+      <c r="B57" s="7"/>
+      <c r="D57" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="E57" s="7"/>
-      <c r="G57" s="9"/>
+      <c r="E57" s="6"/>
+      <c r="G57" s="7"/>
     </row>
     <row r="58" spans="2:7">
-      <c r="B58" s="10" t="s">
+      <c r="B58" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D58" s="20" t="s">
+      <c r="D58" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="E58" s="7"/>
-      <c r="G58" s="8" t="s">
+      <c r="E58" s="6"/>
+      <c r="G58" s="28" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="59" spans="2:7">
-      <c r="B59" s="15" t="s">
+      <c r="B59" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="D59" s="30" t="s">
+      <c r="D59" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="E59" s="7"/>
-      <c r="G59" s="8" t="s">
+      <c r="E59" s="6"/>
+      <c r="G59" s="28" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="60" spans="2:7">
-      <c r="B60" s="9"/>
-      <c r="D60" s="30" t="s">
+      <c r="B60" s="7"/>
+      <c r="D60" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="E60" s="7"/>
-      <c r="G60" s="9"/>
+      <c r="E60" s="6"/>
+      <c r="G60" s="7"/>
     </row>
     <row r="61" spans="2:7">
-      <c r="B61" s="10" t="s">
+      <c r="B61" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D61" s="20" t="s">
+      <c r="D61" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="E61" s="7"/>
-      <c r="G61" s="10" t="s">
+      <c r="E61" s="6"/>
+      <c r="G61" s="5" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="62" spans="2:7">
-      <c r="B62" s="15" t="s">
+      <c r="B62" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="D62" s="20"/>
-      <c r="E62" s="7"/>
-      <c r="G62" s="8" t="s">
+      <c r="D62" s="17"/>
+      <c r="E62" s="6"/>
+      <c r="G62" s="28" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="63" spans="2:7">
-      <c r="B63" s="9"/>
-      <c r="D63" s="23" t="s">
+      <c r="B63" s="7"/>
+      <c r="D63" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="E63" s="7"/>
-      <c r="G63" s="8" t="s">
+      <c r="E63" s="6"/>
+      <c r="G63" s="28" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="64" spans="2:7">
-      <c r="B64" s="10" t="s">
+      <c r="B64" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D64" s="20" t="s">
+      <c r="D64" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="E64" s="7"/>
-      <c r="G64" s="9"/>
+      <c r="E64" s="6"/>
+      <c r="G64" s="7"/>
     </row>
     <row r="65" spans="2:7">
-      <c r="B65" s="15" t="s">
+      <c r="B65" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="D65" s="30" t="s">
+      <c r="D65" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="E65" s="7"/>
-      <c r="G65" s="10" t="s">
+      <c r="E65" s="6"/>
+      <c r="G65" s="5" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="66" spans="2:7">
-      <c r="B66" s="9"/>
-      <c r="D66" s="30" t="s">
+      <c r="B66" s="7"/>
+      <c r="D66" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="E66" s="7"/>
-      <c r="G66" s="8" t="s">
+      <c r="E66" s="6"/>
+      <c r="G66" s="28" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="67" spans="2:7">
-      <c r="B67" s="10" t="s">
+      <c r="B67" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D67" s="20" t="s">
+      <c r="D67" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="E67" s="7"/>
-      <c r="G67" s="8" t="s">
+      <c r="E67" s="6"/>
+      <c r="G67" s="28" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="68" spans="2:7">
-      <c r="B68" s="15" t="s">
+      <c r="B68" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="D68" s="30" t="s">
+      <c r="D68" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="E68" s="7"/>
-      <c r="G68" s="9" t="s">
+      <c r="E68" s="6"/>
+      <c r="G68" s="38" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="69" spans="2:7">
-      <c r="B69" s="9"/>
-      <c r="D69" s="30" t="s">
+      <c r="B69" s="7"/>
+      <c r="D69" s="37"/>
+      <c r="E69" s="6"/>
+      <c r="G69" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="E69" s="7"/>
-      <c r="G69" s="8" t="s">
+    </row>
+    <row r="70" spans="2:7">
+      <c r="B70" s="5" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="70" spans="2:7">
-      <c r="B70" s="10" t="s">
+      <c r="D70" s="22"/>
+      <c r="E70" s="6"/>
+      <c r="G70" s="38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7">
+      <c r="B71" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="D70" s="30"/>
-      <c r="E70" s="7"/>
-      <c r="G70" s="9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="71" spans="2:7">
-      <c r="B71" s="15" t="s">
+      <c r="D71" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="D71" s="23" t="s">
+      <c r="E71" s="6"/>
+      <c r="G71" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="E71" s="7"/>
-      <c r="G71" s="8" t="s">
+    </row>
+    <row r="72" spans="2:7">
+      <c r="B72" s="32" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="72" spans="2:7">
-      <c r="B72" s="15" t="s">
+      <c r="D72" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="D72" s="30" t="s">
+      <c r="E72" s="6"/>
+      <c r="G72" s="7"/>
+    </row>
+    <row r="73" spans="2:7">
+      <c r="B73" s="12"/>
+      <c r="D73" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="E72" s="7"/>
-      <c r="G72" s="9"/>
-    </row>
-    <row r="73" spans="2:7">
-      <c r="B73" s="15"/>
-      <c r="D73" s="20" t="s">
+      <c r="E73" s="6"/>
+      <c r="G73" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="E73" s="7"/>
-      <c r="G73" s="10" t="s">
+    </row>
+    <row r="74" spans="2:7">
+      <c r="B74" s="12"/>
+      <c r="D74" s="37" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="74" spans="2:7">
-      <c r="B74" s="17"/>
-      <c r="D74" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="E74" s="7"/>
-      <c r="G74" s="8" t="s">
+      <c r="E74" s="6"/>
+      <c r="G74" s="28" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="75" spans="2:7">
-      <c r="D75" s="30"/>
-      <c r="E75" s="7"/>
-      <c r="G75" s="8" t="s">
+      <c r="B75" s="12"/>
+      <c r="D75" s="22"/>
+      <c r="E75" s="6"/>
+      <c r="G75" s="28" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="2:7">
-      <c r="D76" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="E76" s="7"/>
-      <c r="G76" s="9"/>
+      <c r="B76" s="12"/>
+      <c r="D76" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="E76" s="6"/>
+      <c r="G76" s="7"/>
     </row>
     <row r="77" spans="2:7">
-      <c r="D77" s="20" t="s">
+      <c r="B77" s="12"/>
+      <c r="D77" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="E77" s="7"/>
-      <c r="G77" s="9"/>
+      <c r="E77" s="6"/>
+      <c r="G77" s="7"/>
     </row>
     <row r="78" spans="2:7">
-      <c r="D78" s="30" t="s">
+      <c r="B78" s="12"/>
+      <c r="D78" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="E78" s="7"/>
-      <c r="G78" s="9"/>
+      <c r="E78" s="6"/>
+      <c r="G78" s="7"/>
     </row>
     <row r="79" spans="2:7">
-      <c r="D79" s="21"/>
-      <c r="E79" s="13"/>
-      <c r="G79" s="17"/>
-    </row>
-    <row r="82" spans="2:4">
-      <c r="B82" s="3" t="s">
+      <c r="B79" s="14"/>
+      <c r="D79" s="18"/>
+      <c r="E79" s="11"/>
+      <c r="G79" s="14"/>
+    </row>
+    <row r="82" spans="2:7">
+      <c r="B82" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="D82" s="3" t="s">
+      <c r="D82" s="46" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="83" spans="2:4">
-      <c r="B83" s="9"/>
-      <c r="D83" s="9"/>
-    </row>
-    <row r="84" spans="2:4">
-      <c r="B84" s="10" t="s">
+      <c r="E82" s="46"/>
+      <c r="G82" s="41" t="s">
         <v>135</v>
       </c>
-      <c r="D84" s="10" t="s">
+    </row>
+    <row r="83" spans="2:7">
+      <c r="B83" s="7"/>
+      <c r="D83" s="17"/>
+      <c r="E83" s="6"/>
+      <c r="G83" s="7"/>
+    </row>
+    <row r="84" spans="2:7">
+      <c r="B84" s="5" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="85" spans="2:4">
-      <c r="B85" s="10" t="s">
+      <c r="D84" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="D85" s="10"/>
-    </row>
-    <row r="86" spans="2:4">
-      <c r="B86" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="D86" s="15" t="s">
+      <c r="E84" s="6"/>
+      <c r="G84" s="5"/>
+    </row>
+    <row r="85" spans="2:7">
+      <c r="B85" s="5" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="87" spans="2:4">
-      <c r="B87" s="15" t="s">
+      <c r="D85" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="D87" s="15" t="s">
+      <c r="E85" s="6"/>
+      <c r="G85" s="32"/>
+    </row>
+    <row r="86" spans="2:7">
+      <c r="B86" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="D86" s="37" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="88" spans="2:4">
-      <c r="B88" s="10"/>
-      <c r="D88" s="15" t="s">
+      <c r="E86" s="6"/>
+      <c r="G86" s="32"/>
+    </row>
+    <row r="87" spans="2:7">
+      <c r="B87" s="32" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="89" spans="2:4">
-      <c r="B89" s="10" t="s">
+      <c r="D87" s="37" t="s">
         <v>142</v>
       </c>
-      <c r="D89" s="15" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="90" spans="2:4">
-      <c r="B90" s="15" t="s">
+      <c r="E87" s="6"/>
+      <c r="G87" s="32"/>
+    </row>
+    <row r="88" spans="2:7">
+      <c r="B88" s="28"/>
+      <c r="D88" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="E88" s="6"/>
+      <c r="G88" s="32"/>
+    </row>
+    <row r="89" spans="2:7">
+      <c r="B89" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D89" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="E89" s="6"/>
+      <c r="G89" s="32"/>
+    </row>
+    <row r="90" spans="2:7">
+      <c r="B90" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="D90" s="15" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="91" spans="2:4">
-      <c r="B91" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="D91" s="15" t="s">
+      <c r="D90" s="37" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="92" spans="2:4">
-      <c r="B92" s="15"/>
-      <c r="D92" s="15" t="s">
+      <c r="E90" s="6"/>
+      <c r="G90" s="32"/>
+    </row>
+    <row r="91" spans="2:7">
+      <c r="B91" s="32" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="93" spans="2:4">
-      <c r="B93" s="10" t="s">
+      <c r="D91" s="37" t="s">
         <v>147</v>
       </c>
-      <c r="D93" s="10"/>
-    </row>
-    <row r="94" spans="2:4">
-      <c r="B94" s="10" t="s">
+      <c r="E91" s="6"/>
+      <c r="G91" s="32"/>
+    </row>
+    <row r="92" spans="2:7">
+      <c r="B92" s="32"/>
+      <c r="D92" s="37"/>
+      <c r="E92" s="6"/>
+      <c r="G92" s="32"/>
+    </row>
+    <row r="93" spans="2:7">
+      <c r="B93" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D94" s="10"/>
-    </row>
-    <row r="95" spans="2:4">
-      <c r="B95" s="15" t="s">
+      <c r="D93" s="40"/>
+      <c r="E93" s="6"/>
+      <c r="G93" s="8"/>
+    </row>
+    <row r="94" spans="2:7">
+      <c r="B94" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D94" s="40"/>
+      <c r="E94" s="6"/>
+      <c r="G94" s="8"/>
+    </row>
+    <row r="95" spans="2:7">
+      <c r="B95" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="D95" s="15"/>
-    </row>
-    <row r="96" spans="2:4">
-      <c r="B96" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="D96" s="15"/>
-    </row>
-    <row r="97" spans="2:4">
-      <c r="B97" s="9"/>
-      <c r="D97" s="9"/>
-    </row>
-    <row r="98" spans="2:4">
-      <c r="B98" s="10" t="s">
+      <c r="D95" s="22"/>
+      <c r="E95" s="6"/>
+      <c r="G95" s="12"/>
+    </row>
+    <row r="96" spans="2:7">
+      <c r="B96" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="D98" s="10"/>
-    </row>
-    <row r="99" spans="2:4">
-      <c r="B99" s="15" t="s">
+      <c r="D96" s="22"/>
+      <c r="E96" s="6"/>
+      <c r="G96" s="12"/>
+    </row>
+    <row r="97" spans="2:7">
+      <c r="B97" s="39"/>
+      <c r="D97" s="17"/>
+      <c r="E97" s="6"/>
+      <c r="G97" s="7"/>
+    </row>
+    <row r="98" spans="2:7">
+      <c r="B98" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D98" s="40"/>
+      <c r="E98" s="6"/>
+      <c r="G98" s="8"/>
+    </row>
+    <row r="99" spans="2:7">
+      <c r="B99" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="D99" s="15"/>
-    </row>
-    <row r="100" spans="2:4">
-      <c r="B100" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="D100" s="15"/>
-    </row>
-    <row r="101" spans="2:4">
-      <c r="B101" s="15"/>
-      <c r="D101" s="15"/>
-    </row>
-    <row r="102" spans="2:4">
-      <c r="B102" s="10" t="s">
+      <c r="D99" s="22"/>
+      <c r="E99" s="6"/>
+      <c r="G99" s="12"/>
+    </row>
+    <row r="100" spans="2:7">
+      <c r="B100" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="D102" s="10"/>
-    </row>
-    <row r="103" spans="2:4">
-      <c r="B103" s="15" t="s">
+      <c r="D100" s="22"/>
+      <c r="E100" s="6"/>
+      <c r="G100" s="12"/>
+    </row>
+    <row r="101" spans="2:7">
+      <c r="B101" s="32"/>
+      <c r="D101" s="22"/>
+      <c r="E101" s="6"/>
+      <c r="G101" s="12"/>
+    </row>
+    <row r="102" spans="2:7">
+      <c r="B102" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D102" s="40"/>
+      <c r="E102" s="6"/>
+      <c r="G102" s="8"/>
+    </row>
+    <row r="103" spans="2:7">
+      <c r="B103" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="D103" s="15"/>
-    </row>
-    <row r="104" spans="2:4">
-      <c r="B104" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="D104" s="15"/>
-    </row>
-    <row r="105" spans="2:4">
-      <c r="B105" s="15" t="s">
+      <c r="D103" s="22"/>
+      <c r="E103" s="6"/>
+      <c r="G103" s="12"/>
+    </row>
+    <row r="104" spans="2:7">
+      <c r="B104" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="D104" s="22"/>
+      <c r="E104" s="6"/>
+      <c r="G104" s="12"/>
+    </row>
+    <row r="105" spans="2:7">
+      <c r="B105" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="D105" s="15"/>
-    </row>
-    <row r="106" spans="2:4">
-      <c r="B106" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="D106" s="15"/>
-    </row>
-    <row r="107" spans="2:4">
-      <c r="B107" s="15"/>
-      <c r="D107" s="15"/>
-    </row>
-    <row r="108" spans="2:4">
-      <c r="B108" s="10" t="s">
+      <c r="D105" s="22"/>
+      <c r="E105" s="6"/>
+      <c r="G105" s="12"/>
+    </row>
+    <row r="106" spans="2:7">
+      <c r="B106" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="D108" s="10"/>
-    </row>
-    <row r="109" spans="2:4">
-      <c r="B109" s="9" t="s">
+      <c r="D106" s="22"/>
+      <c r="E106" s="6"/>
+      <c r="G106" s="12"/>
+    </row>
+    <row r="107" spans="2:7">
+      <c r="B107" s="32"/>
+      <c r="D107" s="22"/>
+      <c r="E107" s="6"/>
+      <c r="G107" s="12"/>
+    </row>
+    <row r="108" spans="2:7">
+      <c r="B108" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="D109" s="9"/>
-    </row>
-    <row r="110" spans="2:4">
-      <c r="B110" s="15" t="s">
+      <c r="D108" s="40"/>
+      <c r="E108" s="6"/>
+      <c r="G108" s="8"/>
+    </row>
+    <row r="109" spans="2:7">
+      <c r="B109" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="D109" s="17"/>
+      <c r="E109" s="6"/>
+      <c r="G109" s="7"/>
+    </row>
+    <row r="110" spans="2:7">
+      <c r="B110" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="D110" s="15"/>
-    </row>
-    <row r="111" spans="2:4">
-      <c r="B111" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="D111" s="15"/>
-    </row>
-    <row r="112" spans="2:4">
-      <c r="B112" s="15" t="s">
+      <c r="D110" s="22"/>
+      <c r="E110" s="6"/>
+      <c r="G110" s="12"/>
+    </row>
+    <row r="111" spans="2:7">
+      <c r="B111" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="D111" s="22"/>
+      <c r="E111" s="6"/>
+      <c r="G111" s="12"/>
+    </row>
+    <row r="112" spans="2:7">
+      <c r="B112" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="D112" s="15"/>
-    </row>
-    <row r="113" spans="2:4">
-      <c r="B113" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="D113" s="15"/>
-    </row>
-    <row r="114" spans="2:4">
-      <c r="B114" s="9"/>
-      <c r="D114" s="9"/>
-    </row>
-    <row r="115" spans="2:4">
-      <c r="B115" s="10" t="s">
+      <c r="D112" s="22"/>
+      <c r="E112" s="6"/>
+      <c r="G112" s="12"/>
+    </row>
+    <row r="113" spans="2:7">
+      <c r="B113" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="D115" s="10"/>
-    </row>
-    <row r="116" spans="2:4">
-      <c r="B116" s="15" t="s">
+      <c r="D113" s="22"/>
+      <c r="E113" s="6"/>
+      <c r="G113" s="12"/>
+    </row>
+    <row r="114" spans="2:7">
+      <c r="B114" s="39"/>
+      <c r="D114" s="17"/>
+      <c r="E114" s="6"/>
+      <c r="G114" s="7"/>
+    </row>
+    <row r="115" spans="2:7">
+      <c r="B115" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D115" s="40"/>
+      <c r="E115" s="6"/>
+      <c r="G115" s="8"/>
+    </row>
+    <row r="116" spans="2:7">
+      <c r="B116" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="D116" s="15"/>
-    </row>
-    <row r="117" spans="2:4">
-      <c r="B117" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="D117" s="15"/>
-    </row>
-    <row r="118" spans="2:4">
-      <c r="B118" s="15" t="s">
+      <c r="D116" s="22"/>
+      <c r="E116" s="6"/>
+      <c r="G116" s="12"/>
+    </row>
+    <row r="117" spans="2:7">
+      <c r="B117" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="D117" s="22"/>
+      <c r="E117" s="6"/>
+      <c r="G117" s="12"/>
+    </row>
+    <row r="118" spans="2:7">
+      <c r="B118" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="D118" s="15"/>
-    </row>
-    <row r="119" spans="2:4">
-      <c r="B119" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="D119" s="15"/>
-    </row>
-    <row r="120" spans="2:4">
-      <c r="B120" s="15" t="s">
+      <c r="D118" s="22"/>
+      <c r="E118" s="6"/>
+      <c r="G118" s="12"/>
+    </row>
+    <row r="119" spans="2:7">
+      <c r="B119" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="D119" s="22"/>
+      <c r="E119" s="6"/>
+      <c r="G119" s="12"/>
+    </row>
+    <row r="120" spans="2:7">
+      <c r="B120" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="D120" s="15"/>
-    </row>
-    <row r="121" spans="2:4">
-      <c r="B121" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="D121" s="15"/>
-    </row>
-    <row r="122" spans="2:4">
-      <c r="B122" s="15" t="s">
+      <c r="D120" s="22"/>
+      <c r="E120" s="6"/>
+      <c r="G120" s="12"/>
+    </row>
+    <row r="121" spans="2:7">
+      <c r="B121" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="D122" s="15"/>
-    </row>
-    <row r="123" spans="2:4">
-      <c r="B123" s="17"/>
-      <c r="D123" s="17"/>
+      <c r="D121" s="22"/>
+      <c r="E121" s="6"/>
+      <c r="G121" s="12"/>
+    </row>
+    <row r="122" spans="2:7">
+      <c r="B122" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="D122" s="22"/>
+      <c r="E122" s="6"/>
+      <c r="G122" s="12"/>
+    </row>
+    <row r="123" spans="2:7">
+      <c r="B123" s="14"/>
+      <c r="D123" s="18"/>
+      <c r="E123" s="11"/>
+      <c r="G123" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D82:E82"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>